<commit_message>
Aggiunto spazio per una colonna "Altro"
</commit_message>
<xml_diff>
--- a/registro.xlsx
+++ b/registro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denic\Documents\Repositories\c++\altro\EsportazioneFatture\builds\builds-EsportazioneFatture\build-EsportazioneFatture-Desktop_Qt_5_15_0_MinGW_32_bit-Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denic\Documents\Repositories\c++\altro\EsportazioneFatture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0684D758-CC98-43EE-912C-1DDB4FAFA902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CCE64A-17FB-40DB-9DEA-EAF9B3384036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Descrizione</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Altro</t>
   </si>
 </sst>
 </file>
@@ -654,7 +657,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,11 +666,10 @@
     <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
     <col min="3" max="6" width="14.7109375" style="1"/>
     <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16" width="14.7109375" style="1"/>
-    <col min="18" max="16384" width="14.7109375" style="1"/>
+    <col min="8" max="16384" width="14.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
@@ -706,8 +708,11 @@
         <v>12</v>
       </c>
       <c r="P1" s="13"/>
-    </row>
-    <row r="2" spans="1:16" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="Q1" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -744,8 +749,9 @@
       <c r="P2" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q2" s="15"/>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -762,8 +768,9 @@
       <c r="N3" s="6"/>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -780,8 +787,9 @@
       <c r="N4" s="10"/>
       <c r="O4" s="9"/>
       <c r="P4" s="10"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q4" s="7"/>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -798,8 +806,9 @@
       <c r="N5" s="10"/>
       <c r="O5" s="9"/>
       <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -816,8 +825,9 @@
       <c r="N6" s="10"/>
       <c r="O6" s="9"/>
       <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -834,8 +844,9 @@
       <c r="N7" s="10"/>
       <c r="O7" s="9"/>
       <c r="P7" s="10"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -852,8 +863,9 @@
       <c r="N8" s="10"/>
       <c r="O8" s="9"/>
       <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -870,8 +882,9 @@
       <c r="N9" s="10"/>
       <c r="O9" s="9"/>
       <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -888,8 +901,9 @@
       <c r="N10" s="10"/>
       <c r="O10" s="9"/>
       <c r="P10" s="10"/>
-    </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -906,8 +920,9 @@
       <c r="N11" s="10"/>
       <c r="O11" s="9"/>
       <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -924,8 +939,9 @@
       <c r="N12" s="10"/>
       <c r="O12" s="9"/>
       <c r="P12" s="10"/>
-    </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -942,8 +958,9 @@
       <c r="N13" s="10"/>
       <c r="O13" s="9"/>
       <c r="P13" s="10"/>
-    </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -960,8 +977,9 @@
       <c r="N14" s="10"/>
       <c r="O14" s="9"/>
       <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -978,8 +996,9 @@
       <c r="N15" s="10"/>
       <c r="O15" s="9"/>
       <c r="P15" s="10"/>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -996,8 +1015,9 @@
       <c r="N16" s="10"/>
       <c r="O16" s="9"/>
       <c r="P16" s="10"/>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1014,8 +1034,9 @@
       <c r="N17" s="10"/>
       <c r="O17" s="9"/>
       <c r="P17" s="10"/>
-    </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1032,8 +1053,9 @@
       <c r="N18" s="10"/>
       <c r="O18" s="9"/>
       <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1050,8 +1072,9 @@
       <c r="N19" s="10"/>
       <c r="O19" s="9"/>
       <c r="P19" s="10"/>
-    </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1068,8 +1091,9 @@
       <c r="N20" s="10"/>
       <c r="O20" s="9"/>
       <c r="P20" s="10"/>
-    </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1086,8 +1110,9 @@
       <c r="N21" s="10"/>
       <c r="O21" s="9"/>
       <c r="P21" s="10"/>
-    </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1104,8 +1129,9 @@
       <c r="N22" s="10"/>
       <c r="O22" s="9"/>
       <c r="P22" s="10"/>
-    </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1122,8 +1148,9 @@
       <c r="N23" s="10"/>
       <c r="O23" s="9"/>
       <c r="P23" s="10"/>
-    </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q23" s="7"/>
+    </row>
+    <row r="24" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1140,8 +1167,9 @@
       <c r="N24" s="10"/>
       <c r="O24" s="9"/>
       <c r="P24" s="10"/>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1158,8 +1186,9 @@
       <c r="N25" s="10"/>
       <c r="O25" s="9"/>
       <c r="P25" s="10"/>
-    </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q25" s="7"/>
+    </row>
+    <row r="26" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1176,8 +1205,9 @@
       <c r="N26" s="10"/>
       <c r="O26" s="9"/>
       <c r="P26" s="10"/>
-    </row>
-    <row r="27" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q26" s="7"/>
+    </row>
+    <row r="27" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1194,8 +1224,9 @@
       <c r="N27" s="10"/>
       <c r="O27" s="9"/>
       <c r="P27" s="10"/>
-    </row>
-    <row r="28" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q27" s="7"/>
+    </row>
+    <row r="28" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1212,8 +1243,9 @@
       <c r="N28" s="10"/>
       <c r="O28" s="9"/>
       <c r="P28" s="10"/>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q28" s="7"/>
+    </row>
+    <row r="29" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1230,8 +1262,9 @@
       <c r="N29" s="10"/>
       <c r="O29" s="9"/>
       <c r="P29" s="10"/>
-    </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q29" s="7"/>
+    </row>
+    <row r="30" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1248,8 +1281,9 @@
       <c r="N30" s="10"/>
       <c r="O30" s="9"/>
       <c r="P30" s="10"/>
-    </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q30" s="7"/>
+    </row>
+    <row r="31" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1266,8 +1300,9 @@
       <c r="N31" s="10"/>
       <c r="O31" s="9"/>
       <c r="P31" s="10"/>
-    </row>
-    <row r="32" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q31" s="7"/>
+    </row>
+    <row r="32" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1284,8 +1319,9 @@
       <c r="N32" s="10"/>
       <c r="O32" s="9"/>
       <c r="P32" s="10"/>
-    </row>
-    <row r="33" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q32" s="7"/>
+    </row>
+    <row r="33" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1302,8 +1338,9 @@
       <c r="N33" s="10"/>
       <c r="O33" s="9"/>
       <c r="P33" s="10"/>
-    </row>
-    <row r="34" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q33" s="7"/>
+    </row>
+    <row r="34" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1320,8 +1357,9 @@
       <c r="N34" s="10"/>
       <c r="O34" s="9"/>
       <c r="P34" s="10"/>
-    </row>
-    <row r="35" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q34" s="7"/>
+    </row>
+    <row r="35" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1338,8 +1376,9 @@
       <c r="N35" s="10"/>
       <c r="O35" s="9"/>
       <c r="P35" s="10"/>
-    </row>
-    <row r="36" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q35" s="7"/>
+    </row>
+    <row r="36" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1356,8 +1395,9 @@
       <c r="N36" s="10"/>
       <c r="O36" s="9"/>
       <c r="P36" s="10"/>
-    </row>
-    <row r="37" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q36" s="7"/>
+    </row>
+    <row r="37" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1374,8 +1414,9 @@
       <c r="N37" s="10"/>
       <c r="O37" s="9"/>
       <c r="P37" s="10"/>
-    </row>
-    <row r="38" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="Q37" s="7"/>
+    </row>
+    <row r="38" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>7</v>
       </c>
@@ -1394,12 +1435,14 @@
       <c r="N38" s="12"/>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
-    </row>
-    <row r="39" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:16" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
+      <c r="Q38" s="11"/>
+    </row>
+    <row r="39" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:17" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>

</xml_diff>